<commit_message>
chg: Added tgt folder for SRNTGT074. Updated SPINS with Risk Estimate Distances (WIP)
</commit_message>
<xml_diff>
--- a/Mission designer/OPAC JFACC Standard Conventional Loads.xlsx
+++ b/Mission designer/OPAC JFACC Standard Conventional Loads.xlsx
@@ -19,7 +19,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="3">'F-16'!$A$1:$K$60</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'F-18C'!$A$1:$I$51</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1727,7 +1727,7 @@
         <xdr:cNvPr id="2" name="Afbeelding 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBC18912-9AA8-3425-780A-72F6F0C863A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BBC18912-9AA8-3425-780A-72F6F0C863A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1739,7 +1739,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1759,7 +1759,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -2300,7 +2300,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3383,7 +3383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
@@ -5118,8 +5118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A6:I51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>